<commit_message>
Changes done to Update framework
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul\IdeaProjects\SeleniumFrameWork\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul.b.gautam\IdeaProjects\SeleniumFrameWorkv2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E246A5D-DB9E-41D8-A0AB-AC7F2A3F631C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA199D95-7687-4E1C-BC86-C78283803E94}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>FirstName</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>rahulgautamvvs@gmail.com</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>TestDATA</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
@@ -66,15 +75,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,14 +97,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -371,45 +403,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E28696EB-5277-44E4-B7BD-C673B03706D3}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{E28696EB-5277-44E4-B7BD-C673B03706D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Reader Data Getting Populated.
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul.b.gautam\IdeaProjects\SeleniumFrameWorkv2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015EEC0E-4A7B-428D-BBBC-21AC22A251E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF2A012-FC69-4ADC-A0CC-7828ABEDA19D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Browser</t>
   </si>
@@ -193,13 +193,25 @@
   </si>
   <si>
     <t>perya</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>TestADBD</t>
+  </si>
+  <si>
+    <t>NOTValidPassword</t>
+  </si>
+  <si>
+    <t>NOTValidUser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,12 +234,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -293,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -324,9 +330,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -616,7 +619,7 @@
   <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +629,8 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="46.140625" customWidth="1"/>
     <col min="5" max="10" width="45.28515625" customWidth="1"/>
-    <col min="11" max="11" width="36.42578125" customWidth="1"/>
+    <col min="11" max="12" width="36.42578125" customWidth="1"/>
+    <col min="13" max="13" width="43.85546875" customWidth="1"/>
     <col min="15" max="15" width="38.42578125" customWidth="1"/>
     <col min="16" max="16" width="28" customWidth="1"/>
     <col min="17" max="17" width="27.7109375" customWidth="1"/>
@@ -741,7 +745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -775,8 +779,6 @@
       <c r="K2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -798,19 +800,29 @@
       <c r="AF2" s="7"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="L3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="7"/>
+      <c r="L4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="N4" s="7" t="s">
         <v>52</v>
       </c>
@@ -872,7 +884,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>37</v>
       </c>
@@ -886,7 +898,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="12"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
@@ -910,7 +922,7 @@
       <c r="AG5" s="7"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -940,7 +952,7 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -970,7 +982,7 @@
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>